<commit_message>
Add Ke Sat, Vietnam
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada-Coimbra-extra_info.xlsx
+++ b/notebooks/jesuita-entrada-Coimbra-extra_info.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "ou 15600325 ou Coimbra, 25-03-1560 MMHM"}, "value": {"comment": "Domingues &amp; O Neil, IV: 2645. MMHM:p.226", "original": "?"}}</t>
+          <t>extra_info: {"date": {"comment": "ou 15600325 ou Coimbra, 25-03-1560 MMHM"}, "value": {"comment": "@wikidata:Q45412 Domingues &amp; O Neil, IV: 2645. MMHM:p.226", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "Schutte, Monumenta historica japoniae I.,p.1180", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 Schutte, Monumenta historica japoniae I.,p.1180", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Corrigido: local de entrada extra_info: {"value": {"comment": "Em Coimbra no ano de 1582 segundo a Carta Annua de 1623 BA", "original": "?"}}</t>
+          <t>Corrigido: local de entrada extra_info: {"value": {"comment": "@wikidata:Q45412 Em Coimbra no ano de 1582 segundo a Carta Annua de 1623 BA", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "MMHM:p.94 (ARSI Japsin 35 13)", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 MMHM:p.94 (ARSI Japsin 35 13)", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "Segundo Dominguez &amp; O Neil, V.III,p.2961. Franco Imagem...Coimbra,II,4,c.36,p.575", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 Segundo Dominguez &amp; O Neil, V.III,p.2961. Franco Imagem...Coimbra,II,4,c.36,p.575", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "Segungo Dominguez, J. M., &amp; O\u2019Neill, C. (2001) II, 1113", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 Segungo Dominguez, J. M., &amp; O\u2019Neill, C. (2001) II, 1113", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "Dehergne n\u00e3o especifica local, Brockey estudos Filosofia e Teologia em Coimbra", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 Dehergne n\u00e3o especifica local, Brockey estudos Filosofia e Teologia em Coimbra", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -672,7 +672,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "ou 16090502"}, "value": {"comment": "(Franco, 1719, t.II, p. 612)", "original": "?"}}</t>
+          <t>extra_info: {"date": {"comment": "ou 16090502"}, "value": {"comment": "@wikidata:Q45412 (Franco, 1719, t.II, p. 612)", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "MMHM:p.8"}, "value": {"comment": "[Adicionado a partir de Franco, Imagem...Coimbra, II, 522", "original": "?"}}</t>
+          <t>extra_info: {"date": {"comment": "MMHM:p.8"}, "value": {"comment": "[Adicionado a partir de Franco, Imagem...Coimbra, II, 522] @wikidata:Q45412", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "\"\"\"Franco, Imagem...Coimbra, v.2 p.616; Barbosa Machado, v.3\"\"\"", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 \"\"\"Franco, Imagem...Coimbra, v.2 p.616; Barbosa Machado, v.3\"\"\"", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "MMHM:p.205 (Sebastian da Maia, da Maya, d'Amaya)", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 MMHM:p.205 (Sebastian da Maia, da Maya, d'Amaya)", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "Segundo Louis Buglio 1688", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 Segundo Louis Buglio 1688", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "MMHM:p.203 (Matias d'Amaia), Schutte, Monumenta historica japoniae I.1234", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 MMHM:p.203 (Matias d'Amaia), Schutte, Monumenta historica japoniae I.1234", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "Ver Brockey, p.230 cit. Carta de A.P. a Viteleschi, de Coimbra, 26 Agosto 1640", "original": "?"}}</t>
+          <t>extra_info: {"value": {"comment": "@wikidata:Q45412 Ver Brockey, p.230 cit. Carta de A.P. a Viteleschi, de Coimbra, 26 Agosto 1640", "original": "?"}}</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[Brockey diz "educated at the College of Coimbra" cap.6 nota 95, citando a carta ânua de 1656, Ajuda, 49-V.14:62v] extra_info: {"value": {"comment": "Brockey, cap.6 n.95", "original": "?"}}</t>
+          <t>[Brockey diz "educated at the College of Coimbra" cap.6 nota 95, citando a carta ânua de 1656, Ajuda, 49-V.14:62v] extra_info: {"value": {"comment": "@wikidata:Q45412 Brockey, cap.6 n.95", "original": "?"}}</t>
         </is>
       </c>
     </row>

</xml_diff>